<commit_message>
Ula: Excel files changed
</commit_message>
<xml_diff>
--- a/src/Dataset/EXCEL.xlsx
+++ b/src/Dataset/EXCEL.xlsx
@@ -27,9 +27,6 @@
     <t>Odds</t>
   </si>
   <si>
-    <t>Benefit</t>
-  </si>
-  <si>
     <t>Express</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t>Kabrera-Yuan 2 win</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -84,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -391,7 +392,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,12 +411,12 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -423,13 +424,13 @@
       <c r="C2" s="1">
         <v>2.8</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>78</v>
@@ -437,13 +438,13 @@
       <c r="C3" s="1">
         <v>1.4</v>
       </c>
-      <c r="D3">
-        <v>110</v>
+      <c r="D3" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>69</v>
@@ -451,13 +452,13 @@
       <c r="C4" s="1">
         <v>16.2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -465,13 +466,13 @@
       <c r="C5" s="1">
         <v>9.25</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>70</v>
@@ -479,13 +480,13 @@
       <c r="C6" s="1">
         <v>3.2857142857142856</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>100</v>
@@ -493,13 +494,13 @@
       <c r="C7" s="1">
         <v>2.5</v>
       </c>
-      <c r="D7" s="1">
-        <v>247.25</v>
+      <c r="D7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>100</v>
@@ -507,13 +508,13 @@
       <c r="C8" s="1">
         <v>3.1666666666666665</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>43</v>
@@ -521,13 +522,13 @@
       <c r="C9" s="1">
         <v>2.2222222222222223</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -535,13 +536,13 @@
       <c r="C10" s="1">
         <v>2.1428571428571428</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>100</v>
@@ -549,13 +550,13 @@
       <c r="C11" s="1">
         <v>3.25</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -563,13 +564,13 @@
       <c r="C12" s="1">
         <v>2.1666666666666665</v>
       </c>
-      <c r="D12">
-        <v>218</v>
+      <c r="D12" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -577,13 +578,13 @@
       <c r="C13" s="1">
         <v>5.1428571428571432</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>100</v>
@@ -591,13 +592,13 @@
       <c r="C14" s="1">
         <v>7.2857142857142856</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>50</v>
@@ -605,12 +606,13 @@
       <c r="C15" s="1">
         <v>1.7142857142857144</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>